<commit_message>
Add test cases for XSSFTableColumn
</commit_message>
<xml_diff>
--- a/testcases/test-data/spreadsheet/CustomXMLMappings-complex-type.xlsx
+++ b/testcases/test-data/spreadsheet/CustomXMLMappings-complex-type.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lka\git\poi\test-data\spreadsheet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="7695" windowHeight="5730"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="7695" windowHeight="5730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -67,14 +72,28 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>Unmapped Column</t>
+  </si>
+  <si>
+    <t>[This text should be cleared if the table expands]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -102,17 +121,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -320,12 +348,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabella2" displayName="Tabella2" ref="C5:E9" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="C5:E9"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabella2" displayName="Tabella2" ref="C5:F9" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="C5:F9"/>
+  <tableColumns count="4">
     <tableColumn id="1" uniqueName="ID" name="ID">
       <xmlColumnPr mapId="2" xpath="/ns1:MapInfo/ns1:Schema/@ID" xmlDataType="string"/>
     </tableColumn>
+    <tableColumn id="4" uniqueName="4" name="Unmapped Column"/>
     <tableColumn id="2" uniqueName="SchemaRef" name="SchemaRef">
       <xmlColumnPr mapId="2" xpath="/ns1:MapInfo/ns1:Schema/@SchemaRef" xmlDataType="string"/>
     </tableColumn>
@@ -348,7 +377,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -390,7 +419,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,9 +451,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -456,6 +503,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -631,20 +696,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="18" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:18">
+    <row r="4" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>0</v>
       </c>
@@ -688,7 +753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="5:18">
+    <row r="5" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E5">
         <v>1</v>
       </c>
@@ -722,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="5:18">
+    <row r="6" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -756,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="5:18">
+    <row r="7" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E7" s="2">
         <v>3</v>
       </c>
@@ -790,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="5:18">
+    <row r="8" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E8" s="2">
         <v>4</v>
       </c>
@@ -824,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="5:18">
+    <row r="9" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E9" s="2">
         <v>5</v>
       </c>
@@ -868,81 +933,94 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="5" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="3:8">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H3" s="1"/>
     </row>
-    <row r="5" spans="3:8">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:8">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="3:8">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <v>2</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="3:8">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <v>3</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="3:8">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>4</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>